<commit_message>
Publish Aerosol for MIROC6.
</commit_message>
<xml_diff>
--- a/cmip6/models/miroc6/cmip6_miroc_miroc6_aerosol.xlsx
+++ b/cmip6/models/miroc6/cmip6_miroc_miroc6_aerosol.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11209"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Documents/work/project/CMIP6/ES-DOC/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE589BC0-6B14-2C45-8923-10EFE7938D27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="7920" yWindow="440" windowWidth="23000" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -17,12 +23,12 @@
     <sheet name="6. Optical Radiative Properties" sheetId="8" r:id="rId8"/>
     <sheet name="7. Model" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="512">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -1507,17 +1513,84 @@
   </si>
   <si>
     <t>STS (supercooled ternary solution aerosol particule)</t>
+  </si>
+  <si>
+    <t>SPRINTARS</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>aerosol transport,aerosol-radiation interaction,aerosol-cloud interaction</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Fortran</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>leap-frog</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>T85L81h</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>radiative forcing</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Observational data on mass concentration of each aerosol comonent and aerosol optical thickness from satellite and in-situ are mainly used to tune the aerosol model. The aerosol radiative frocing which can simulated observed trend of the surface air temperature is also focued as a climate model.</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>aerosol optical thickness,mass concentration,Ångström exponent,aerosol single scattering albedo</t>
+  </si>
+  <si>
+    <t>aerosol optical thickness,mass concentration,Ångström exponent,aerosol single scattering albedo</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>soil dust,sea salt,DMS</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>A half of BC/OC from anthropogenic sources is internally mixed and the others are externally mixed.</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>Spectral Radiation-Transport Model for Aerosol Species (SPRINTARS) predicts mass mixing ratios of the main tropospheric aerosols which are black carbon (BC), organic matter (OM), sulfate, soil dust, and sea salt, and the precursor gases of sulfate (sulfur dioxide and dimethylsulfide). SPRINTARS calculates not only the aerosol transport processes of emission, advection, diffusion, sulfur chemistry, wet deposition, dry deposition, and gravitational settling, but also the aerosol-radiation and aerosol-cloud interactions by coupled with the radiation and cloud-precipitation schemes in MIROC. See sections on model description in Takemura (2018, http://www.cger.nies.go.jp/publications/report/i138/i138.pdf) for furtther details.</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>/m^3</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>m^2/g</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>The radiative process in MIROC is based on the two-stream discrete ordinate/adding method (Nakajima et al., 2000, doi:10.1364/AO.39.004869). In the radiation scheme, extinction and mass coefficients, asymmetry factor and truncation factor in each band are calculated for aerosols and clouds. The aerosol optical parameters are calculated according to the Mie theory and volume-weighted refractive indices with water for the internal mixture. The wavelength-dependent refractive indices are according to WCP-55 (1983, "Report of the experts meeting on aerosols and their climatic effects") for aerosols and d'Almeida et al. (1991, "Atmospheric Aerosols: Global Climatology and Radiative Characteristics") for water. See section 2.2 in Takemura (2018, http://www.cger.nies.go.jp/publications/report/i138/i138.pdf) for furtther details.</t>
+    <phoneticPr fontId="15"/>
+  </si>
+  <si>
+    <t>A parameterization based on the Köhler theory is introduced for water cloud (Ghan et al., 1997, doi:10.1029/97JD01810; Abdul-Razzak and Ghan, 2000, doi:10.1029/1999JD901161). The cloud droplet effective radius related with the Twomey effect is calculated depending on the prognostic cloud droplet number concentration and cloud water mixing ratio. The Berry's parameterization is adopted for the autoconversion process. The ice crystal number concetration is also treated as a prognostic variable. The homogeneous and heterogeneous freezings are based on Kärcher and Lohmann (2002, doi:10.1029/2001JD000470) and Lohmann and Diehl (2006, doi:10.1175/JAS3662.1), respectively. See section 3.2 in Takemura (2018, http://www.cger.nies.go.jp/publications/report/i138/i138.pdf) for furtther details.</t>
+    <phoneticPr fontId="15"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1614,6 +1687,19 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1659,7 +1745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1703,17 +1789,28 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1755,7 +1852,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1787,9 +1884,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1821,6 +1936,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1996,24 +2129,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="180.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="33">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="20">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2021,7 +2154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="20">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2029,7 +2162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="20">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -2037,7 +2170,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="20">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -2045,7 +2178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="20">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -2053,37 +2186,37 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="20">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="20">
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="20">
       <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="20">
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="20">
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="20">
       <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="18">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -2091,7 +2224,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="18">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -2099,7 +2232,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="18">
       <c r="A18" s="5" t="s">
         <v>21</v>
       </c>
@@ -2107,7 +2240,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="18">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
@@ -2115,41 +2248,44 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="20">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="20">
       <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="15"/>
   <hyperlinks>
-    <hyperlink ref="B16" r:id="rId1"/>
-    <hyperlink ref="B17" r:id="rId2"/>
+    <hyperlink ref="B16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="80.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="80.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30">
       <c r="A1" s="7" t="s">
         <v>27</v>
       </c>
@@ -2160,7 +2296,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="18">
       <c r="A5" s="9" t="s">
         <v>29</v>
       </c>
@@ -2184,11 +2320,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="18">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="18">
       <c r="A12" s="9" t="s">
         <v>34</v>
       </c>
@@ -2212,39 +2348,40 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="18">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="15"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Top Level,Key Properties,Grid,Transport,Emissions,Concentrations,Optical Radiative Properties,Model"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1"/>
-    <hyperlink ref="A13" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A13" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD145"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AI146"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -2280,7 +2417,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -2307,7 +2446,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="24" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
@@ -2334,7 +2475,9 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="178" customHeight="1">
-      <c r="B16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="18" spans="1:31" ht="24" customHeight="1">
       <c r="A18" s="9" t="s">
@@ -2361,7 +2504,9 @@
       </c>
     </row>
     <row r="21" spans="1:31" ht="24" customHeight="1">
-      <c r="B21" s="11"/>
+      <c r="B21" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="AA21" s="6" t="s">
         <v>61</v>
       </c>
@@ -2378,725 +2523,756 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="24" customHeight="1">
-      <c r="A23" s="9" t="s">
+    <row r="22" spans="1:31" ht="24" customHeight="1">
+      <c r="B22" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB22" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC22" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE22" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" ht="24" customHeight="1">
+      <c r="A24" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B24" s="9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="24" customHeight="1">
-      <c r="A24" s="14" t="s">
+    <row r="25" spans="1:31" ht="24" customHeight="1">
+      <c r="A25" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B25" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C25" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="24" customHeight="1">
-      <c r="B25" s="11"/>
-    </row>
-    <row r="27" spans="1:31" ht="24" customHeight="1">
-      <c r="A27" s="9" t="s">
+    <row r="26" spans="1:31" ht="24" customHeight="1">
+      <c r="B26" s="11" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" ht="24" customHeight="1">
+      <c r="A28" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B28" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="24" customHeight="1">
-      <c r="A28" s="14" t="s">
+    <row r="29" spans="1:31" ht="24" customHeight="1">
+      <c r="A29" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B29" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C29" s="10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="24" customHeight="1">
-      <c r="B29" s="10" t="s">
+    <row r="30" spans="1:31" ht="24" customHeight="1">
+      <c r="B30" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="24" customHeight="1">
-      <c r="B30" s="11"/>
-      <c r="AA30" s="6" t="s">
+    <row r="31" spans="1:31" ht="24" customHeight="1">
+      <c r="B31" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="AB30" s="6" t="s">
+      <c r="AA31" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB31" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AC30" s="6" t="s">
+      <c r="AC31" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="24" customHeight="1">
-      <c r="A32" s="9" t="s">
+    <row r="33" spans="1:3" ht="24" customHeight="1">
+      <c r="A33" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B33" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="24" customHeight="1">
-      <c r="A33" s="14" t="s">
+    <row r="34" spans="1:3" ht="24" customHeight="1">
+      <c r="A34" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B34" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="24" customHeight="1">
-      <c r="B34" s="11"/>
-    </row>
-    <row r="36" spans="1:3" ht="24" customHeight="1">
-      <c r="A36" s="9" t="s">
+    <row r="35" spans="1:3" ht="24" customHeight="1">
+      <c r="B35" s="11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="24" customHeight="1">
+      <c r="A37" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B37" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="24" customHeight="1">
-      <c r="A37" s="14" t="s">
+    <row r="38" spans="1:3" ht="24" customHeight="1">
+      <c r="A38" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B38" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C38" s="10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="24" customHeight="1">
-      <c r="B38" s="11"/>
-    </row>
-    <row r="41" spans="1:3" ht="24" customHeight="1">
-      <c r="A41" s="12" t="s">
+    <row r="39" spans="1:3" ht="24" customHeight="1">
+      <c r="B39" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="24" customHeight="1">
+      <c r="A42" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B42" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="24" customHeight="1">
-      <c r="B42" s="13" t="s">
+    <row r="43" spans="1:3" ht="24" customHeight="1">
+      <c r="B43" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="24" customHeight="1">
-      <c r="A44" s="9" t="s">
+    <row r="45" spans="1:3" ht="24" customHeight="1">
+      <c r="A45" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B45" s="9" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="24" customHeight="1">
-      <c r="A45" s="14" t="s">
+    <row r="46" spans="1:3" ht="24" customHeight="1">
+      <c r="A46" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B46" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C46" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="24" customHeight="1">
-      <c r="B46" s="11"/>
-    </row>
-    <row r="48" spans="1:3" ht="24" customHeight="1">
-      <c r="A48" s="9" t="s">
+    <row r="47" spans="1:3" ht="24" customHeight="1">
+      <c r="B47" s="11"/>
+    </row>
+    <row r="49" spans="1:30" ht="24" customHeight="1">
+      <c r="A49" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B49" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:30" ht="24" customHeight="1">
-      <c r="A49" s="14" t="s">
+    <row r="50" spans="1:30" ht="24" customHeight="1">
+      <c r="A50" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B50" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C50" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:30" ht="24" customHeight="1">
-      <c r="B50" s="11"/>
-    </row>
-    <row r="52" spans="1:30" ht="24" customHeight="1">
-      <c r="A52" s="9" t="s">
+    <row r="51" spans="1:30" ht="24" customHeight="1">
+      <c r="B51" s="11"/>
+    </row>
+    <row r="53" spans="1:30" ht="24" customHeight="1">
+      <c r="A53" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B53" s="9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:30" ht="24" customHeight="1">
-      <c r="A53" s="14" t="s">
+    <row r="54" spans="1:30" ht="24" customHeight="1">
+      <c r="A54" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B54" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C54" s="10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:30" ht="24" customHeight="1">
-      <c r="B54" s="8" t="s">
+    <row r="55" spans="1:30" ht="24" customHeight="1">
+      <c r="B55" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:30" ht="24" customHeight="1">
-      <c r="B55" s="11"/>
-    </row>
-    <row r="58" spans="1:30" ht="24" customHeight="1">
-      <c r="A58" s="12" t="s">
+    <row r="56" spans="1:30" ht="24" customHeight="1">
+      <c r="B56" s="11" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="59" spans="1:30" ht="24" customHeight="1">
+      <c r="A59" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B59" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="1:30" ht="24" customHeight="1">
-      <c r="B59" s="13" t="s">
+    <row r="60" spans="1:30" ht="24" customHeight="1">
+      <c r="B60" s="13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:30" ht="24" customHeight="1">
-      <c r="A61" s="9" t="s">
+    <row r="62" spans="1:30" ht="24" customHeight="1">
+      <c r="A62" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B62" s="9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="62" spans="1:30" ht="24" customHeight="1">
-      <c r="A62" s="14" t="s">
+    <row r="63" spans="1:30" ht="24" customHeight="1">
+      <c r="A63" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B63" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C63" s="10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:30" ht="24" customHeight="1">
-      <c r="B63" s="11"/>
-      <c r="AA63" s="6" t="s">
+    <row r="64" spans="1:30" ht="24" customHeight="1">
+      <c r="B64" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="AB63" s="6" t="s">
+      <c r="AA64" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB64" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="AC63" s="6" t="s">
+      <c r="AC64" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="AD63" s="6" t="s">
+      <c r="AD64" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:35" ht="24" customHeight="1">
-      <c r="A65" s="9" t="s">
+    <row r="66" spans="1:35" ht="24" customHeight="1">
+      <c r="A66" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B66" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="66" spans="1:35" ht="24" customHeight="1">
-      <c r="A66" s="14" t="s">
+    <row r="67" spans="1:35" ht="24" customHeight="1">
+      <c r="A67" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B67" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C67" s="10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="67" spans="1:35" ht="24" customHeight="1">
-      <c r="B67" s="11"/>
-    </row>
-    <row r="69" spans="1:35" ht="24" customHeight="1">
-      <c r="A69" s="9" t="s">
+    <row r="68" spans="1:35" ht="24" customHeight="1">
+      <c r="B68" s="11"/>
+    </row>
+    <row r="70" spans="1:35" ht="24" customHeight="1">
+      <c r="A70" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B70" s="9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:35" ht="24" customHeight="1">
-      <c r="A70" s="14" t="s">
+    <row r="71" spans="1:35" ht="24" customHeight="1">
+      <c r="A71" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B70" s="10" t="s">
+      <c r="B71" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="C71" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="71" spans="1:35" ht="24" customHeight="1">
-      <c r="B71" s="11"/>
-    </row>
-    <row r="73" spans="1:35" ht="24" customHeight="1">
-      <c r="A73" s="9" t="s">
+    <row r="72" spans="1:35" ht="24" customHeight="1">
+      <c r="B72" s="11"/>
+    </row>
+    <row r="74" spans="1:35" ht="24" customHeight="1">
+      <c r="A74" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B74" s="9" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="1:35" ht="24" customHeight="1">
-      <c r="A74" s="14" t="s">
+    <row r="75" spans="1:35" ht="24" customHeight="1">
+      <c r="A75" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B75" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C75" s="10" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="75" spans="1:35" ht="24" customHeight="1">
-      <c r="B75" s="11"/>
-    </row>
-    <row r="77" spans="1:35" ht="24" customHeight="1">
-      <c r="A77" s="9" t="s">
+    <row r="76" spans="1:35" ht="24" customHeight="1">
+      <c r="B76" s="11">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="78" spans="1:35" ht="24" customHeight="1">
+      <c r="A78" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B78" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="78" spans="1:35" ht="24" customHeight="1">
-      <c r="A78" s="14" t="s">
+    <row r="79" spans="1:35" ht="24" customHeight="1">
+      <c r="A79" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B78" s="10" t="s">
+      <c r="B79" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C78" s="10" t="s">
+      <c r="C79" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="79" spans="1:35" ht="24" customHeight="1">
-      <c r="B79" s="11"/>
-      <c r="AA79" s="6" t="s">
+    <row r="80" spans="1:35" ht="24" customHeight="1">
+      <c r="B80" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="AA80" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AB79" s="6" t="s">
+      <c r="AB80" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="AC79" s="6" t="s">
+      <c r="AC80" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="AD79" s="6" t="s">
+      <c r="AD80" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="AE79" s="6" t="s">
+      <c r="AE80" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="AF79" s="6" t="s">
+      <c r="AF80" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="AG79" s="6" t="s">
+      <c r="AG80" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="AH79" s="6" t="s">
+      <c r="AH80" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="AI79" s="6" t="s">
+      <c r="AI80" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="24" customHeight="1">
-      <c r="A82" s="12" t="s">
+    <row r="83" spans="1:3" ht="24" customHeight="1">
+      <c r="A83" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B82" s="12" t="s">
+      <c r="B83" s="12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="24" customHeight="1">
-      <c r="B83" s="13"/>
-    </row>
-    <row r="85" spans="1:3" ht="24" customHeight="1">
-      <c r="A85" s="9" t="s">
+    <row r="84" spans="1:3" ht="24" customHeight="1">
+      <c r="B84" s="13"/>
+    </row>
+    <row r="86" spans="1:3" ht="24" customHeight="1">
+      <c r="A86" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B85" s="9" t="s">
+      <c r="B86" s="9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="24" customHeight="1">
-      <c r="A86" s="14" t="s">
+    <row r="87" spans="1:3" ht="24" customHeight="1">
+      <c r="A87" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B86" s="10" t="s">
+      <c r="B87" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C86" s="10" t="s">
+      <c r="C87" s="10" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="24" customHeight="1">
-      <c r="B87" s="8" t="s">
+    <row r="88" spans="1:3" ht="24" customHeight="1">
+      <c r="B88" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="24" customHeight="1">
-      <c r="B88" s="11"/>
-    </row>
-    <row r="90" spans="1:3" ht="24" customHeight="1">
-      <c r="A90" s="9" t="s">
+    <row r="89" spans="1:3" ht="24" customHeight="1">
+      <c r="B89" s="11"/>
+    </row>
+    <row r="91" spans="1:3" ht="24" customHeight="1">
+      <c r="A91" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B90" s="9" t="s">
+      <c r="B91" s="9" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="24" customHeight="1">
-      <c r="A91" s="14" t="s">
+    <row r="92" spans="1:3" ht="24" customHeight="1">
+      <c r="A92" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B91" s="10" t="s">
+      <c r="B92" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C91" s="10" t="s">
+      <c r="C92" s="10" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="24" customHeight="1">
-      <c r="B92" s="8" t="s">
+    <row r="93" spans="1:3" ht="24" customHeight="1">
+      <c r="B93" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="24" customHeight="1">
-      <c r="B93" s="11"/>
-    </row>
-    <row r="95" spans="1:3" ht="24" customHeight="1">
-      <c r="A95" s="9" t="s">
+    <row r="94" spans="1:3" ht="24" customHeight="1">
+      <c r="B94" s="11"/>
+    </row>
+    <row r="96" spans="1:3" ht="24" customHeight="1">
+      <c r="A96" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B95" s="9" t="s">
+      <c r="B96" s="9" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="24" customHeight="1">
-      <c r="A96" s="14" t="s">
+    <row r="97" spans="1:3" ht="24" customHeight="1">
+      <c r="A97" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B96" s="10" t="s">
+      <c r="B97" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C96" s="10" t="s">
+      <c r="C97" s="10" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="24" customHeight="1">
-      <c r="B97" s="11"/>
-    </row>
-    <row r="100" spans="1:3" ht="24" customHeight="1">
-      <c r="A100" s="12" t="s">
+    <row r="98" spans="1:3" ht="24" customHeight="1">
+      <c r="B98" s="11"/>
+    </row>
+    <row r="101" spans="1:3" ht="24" customHeight="1">
+      <c r="A101" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B100" s="12" t="s">
+      <c r="B101" s="12" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="24" customHeight="1">
-      <c r="B101" s="13" t="s">
+    <row r="102" spans="1:3" ht="24" customHeight="1">
+      <c r="B102" s="13" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="24" customHeight="1">
-      <c r="A103" s="9" t="s">
+    <row r="104" spans="1:3" ht="24" customHeight="1">
+      <c r="A104" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B103" s="9" t="s">
+      <c r="B104" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="24" customHeight="1">
-      <c r="A104" s="14" t="s">
+    <row r="105" spans="1:3" ht="24" customHeight="1">
+      <c r="A105" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B104" s="10" t="s">
+      <c r="B105" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="C104" s="10" t="s">
+      <c r="C105" s="10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="24" customHeight="1">
-      <c r="B105" s="11"/>
-    </row>
-    <row r="107" spans="1:3" ht="24" customHeight="1">
-      <c r="A107" s="9" t="s">
+    <row r="106" spans="1:3" ht="24" customHeight="1">
+      <c r="B106" s="11" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="24" customHeight="1">
+      <c r="A108" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B107" s="9" t="s">
+      <c r="B108" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="24" customHeight="1">
-      <c r="A108" s="14" t="s">
+    <row r="109" spans="1:3" ht="24" customHeight="1">
+      <c r="A109" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B108" s="10" t="s">
+      <c r="B109" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="C108" s="10" t="s">
+      <c r="C109" s="10" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="24" customHeight="1">
-      <c r="B109" s="11"/>
-    </row>
-    <row r="111" spans="1:3" ht="24" customHeight="1">
-      <c r="A111" s="9" t="s">
+    <row r="110" spans="1:3" ht="24" customHeight="1">
+      <c r="B110" s="11"/>
+    </row>
+    <row r="112" spans="1:3" ht="24" customHeight="1">
+      <c r="A112" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B111" s="9" t="s">
+      <c r="B112" s="9" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="24" customHeight="1">
-      <c r="A112" s="14" t="s">
+    <row r="113" spans="1:3" ht="24" customHeight="1">
+      <c r="A113" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B112" s="10" t="s">
+      <c r="B113" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="C112" s="10" t="s">
+      <c r="C113" s="10" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="24" customHeight="1">
-      <c r="B113" s="11"/>
-    </row>
-    <row r="115" spans="1:3" ht="24" customHeight="1">
-      <c r="A115" s="9" t="s">
+    <row r="114" spans="1:3" ht="24" customHeight="1">
+      <c r="B114" s="11"/>
+    </row>
+    <row r="116" spans="1:3" ht="24" customHeight="1">
+      <c r="A116" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B115" s="9" t="s">
+      <c r="B116" s="9" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="24" customHeight="1">
-      <c r="A116" s="14" t="s">
+    <row r="117" spans="1:3" ht="24" customHeight="1">
+      <c r="A117" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B116" s="10" t="s">
+      <c r="B117" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C116" s="10" t="s">
+      <c r="C117" s="10" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="24" customHeight="1">
-      <c r="B117" s="11"/>
-    </row>
-    <row r="119" spans="1:3" ht="24" customHeight="1">
-      <c r="A119" s="9" t="s">
+    <row r="118" spans="1:3" ht="24" customHeight="1">
+      <c r="B118" s="11"/>
+    </row>
+    <row r="120" spans="1:3" ht="24" customHeight="1">
+      <c r="A120" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="B119" s="9" t="s">
+      <c r="B120" s="9" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="24" customHeight="1">
-      <c r="A120" s="14" t="s">
+    <row r="121" spans="1:3" ht="24" customHeight="1">
+      <c r="A121" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B120" s="10" t="s">
+      <c r="B121" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="C120" s="10" t="s">
+      <c r="C121" s="10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="24" customHeight="1">
-      <c r="B121" s="11"/>
-    </row>
-    <row r="124" spans="1:3" ht="24" customHeight="1">
-      <c r="A124" s="12" t="s">
+    <row r="122" spans="1:3" ht="24" customHeight="1">
+      <c r="B122" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="24" customHeight="1">
+      <c r="A125" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B124" s="12" t="s">
+      <c r="B125" s="12" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="24" customHeight="1">
-      <c r="B125" s="13" t="s">
+    <row r="126" spans="1:3" ht="24" customHeight="1">
+      <c r="B126" s="13" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="24" customHeight="1">
-      <c r="A127" s="9" t="s">
+    <row r="128" spans="1:3" ht="24" customHeight="1">
+      <c r="A128" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B127" s="9" t="s">
+      <c r="B128" s="9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="24" customHeight="1">
-      <c r="A128" s="14" t="s">
+    <row r="129" spans="1:3" ht="24" customHeight="1">
+      <c r="A129" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B128" s="10" t="s">
+      <c r="B129" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C128" s="10" t="s">
+      <c r="C129" s="10" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="24" customHeight="1">
-      <c r="B129" s="8" t="s">
+    <row r="130" spans="1:3" ht="24" customHeight="1">
+      <c r="B130" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="178" customHeight="1">
-      <c r="B130" s="11"/>
-    </row>
-    <row r="132" spans="1:3" ht="24" customHeight="1">
-      <c r="A132" s="9" t="s">
+    <row r="131" spans="1:3" ht="178" customHeight="1">
+      <c r="B131" s="11" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="24" customHeight="1">
+      <c r="A133" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="B132" s="9" t="s">
+      <c r="B133" s="9" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="24" customHeight="1">
-      <c r="A133" s="14" t="s">
+    <row r="134" spans="1:3" ht="24" customHeight="1">
+      <c r="A134" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B133" s="10" t="s">
+      <c r="B134" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C133" s="10" t="s">
+      <c r="C134" s="10" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="24" customHeight="1">
-      <c r="B134" s="8" t="s">
+    <row r="135" spans="1:3" ht="24" customHeight="1">
+      <c r="B135" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="24" customHeight="1">
-      <c r="B135" s="11"/>
-    </row>
-    <row r="137" spans="1:3" ht="24" customHeight="1">
-      <c r="A137" s="9" t="s">
+    <row r="136" spans="1:3" ht="24" customHeight="1">
+      <c r="B136" s="11" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="24" customHeight="1">
+      <c r="A138" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="B137" s="9" t="s">
+      <c r="B138" s="9" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="24" customHeight="1">
-      <c r="A138" s="14" t="s">
+    <row r="139" spans="1:3" ht="24" customHeight="1">
+      <c r="A139" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B138" s="10" t="s">
+      <c r="B139" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="C138" s="10" t="s">
+      <c r="C139" s="10" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="24" customHeight="1">
-      <c r="B139" s="8" t="s">
+    <row r="140" spans="1:3" ht="24" customHeight="1">
+      <c r="B140" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="24" customHeight="1">
-      <c r="B140" s="11"/>
-    </row>
-    <row r="142" spans="1:3" ht="24" customHeight="1">
-      <c r="A142" s="9" t="s">
+    <row r="141" spans="1:3" ht="24" customHeight="1">
+      <c r="B141" s="11" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="24" customHeight="1">
+      <c r="A143" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="B142" s="9" t="s">
+      <c r="B143" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="24" customHeight="1">
-      <c r="A143" s="14" t="s">
+    <row r="144" spans="1:3" ht="24" customHeight="1">
+      <c r="A144" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B143" s="10" t="s">
+      <c r="B144" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="C143" s="10" t="s">
+      <c r="C144" s="10" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="24" customHeight="1">
-      <c r="B144" s="8" t="s">
+    <row r="145" spans="2:2" ht="24" customHeight="1">
+      <c r="B145" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="24" customHeight="1">
-      <c r="B145" s="11"/>
+    <row r="146" spans="2:2" ht="24" customHeight="1">
+      <c r="B146" s="11" t="s">
+        <v>503</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21:B22" xr:uid="{7D5E6792-03F0-D54E-9DC1-5EAD689A9EFD}">
       <formula1>AA21:AE21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30">
-      <formula1>AA30:AC30</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31" xr:uid="{00000000-0002-0000-0200-000001000000}">
+      <formula1>AA31:AC31</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35 B118 B114 B98 B76 B72 B68" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39 B122" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63">
-      <formula1>AA63:AD63</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64" xr:uid="{00000000-0002-0000-0200-000004000000}">
+      <formula1>AA64:AD64</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B67">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B71">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79">
-      <formula1>AA79:AI79</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B97">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B113">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B117">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B121">
-      <formula1>"TRUE,FALSE"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80" xr:uid="{00000000-0002-0000-0200-000008000000}">
+      <formula1>AA80:AI80</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3104,17 +3280,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -3199,7 +3375,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
-      <c r="B15" s="11"/>
+      <c r="B15" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="24" customHeight="1">
       <c r="A18" s="12" t="s">
@@ -3234,7 +3412,9 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="24" customHeight="1">
-      <c r="B23" s="11"/>
+      <c r="B23" s="11" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="24" customHeight="1">
       <c r="A25" s="9" t="s">
@@ -3322,21 +3502,18 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
-      <c r="B39" s="11"/>
+      <c r="B39" s="11" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15 B39" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31 B35" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3344,17 +3521,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:AE25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="24" customHeight="1">
@@ -3439,7 +3616,9 @@
       </c>
     </row>
     <row r="15" spans="1:31" ht="24" customHeight="1">
-      <c r="B15" s="11"/>
+      <c r="B15" s="11" t="s">
+        <v>233</v>
+      </c>
       <c r="AA15" s="6" t="s">
         <v>231</v>
       </c>
@@ -3481,7 +3660,9 @@
       </c>
     </row>
     <row r="20" spans="1:31" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>231</v>
+      </c>
       <c r="AA20" s="6" t="s">
         <v>231</v>
       </c>
@@ -3523,7 +3704,9 @@
       </c>
     </row>
     <row r="25" spans="1:31" ht="24" customHeight="1">
-      <c r="B25" s="11"/>
+      <c r="B25" s="11" t="s">
+        <v>247</v>
+      </c>
       <c r="AA25" s="6" t="s">
         <v>231</v>
       </c>
@@ -3538,14 +3721,12 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+  <phoneticPr fontId="15"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15 B20" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>AA15:AE15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
-      <formula1>AA20:AE20</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25" xr:uid="{00000000-0002-0000-0400-000002000000}">
       <formula1>AA25:AD25</formula1>
     </dataValidation>
   </dataValidations>
@@ -3554,17 +3735,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AI58"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="24" customHeight="1">
@@ -3654,7 +3835,9 @@
       </c>
     </row>
     <row r="16" spans="1:33" ht="24" customHeight="1">
-      <c r="B16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA16" s="6" t="s">
         <v>261</v>
       </c>
@@ -3677,237 +3860,514 @@
         <v>65</v>
       </c>
     </row>
+    <row r="17" spans="1:35" ht="24" customHeight="1">
+      <c r="B17" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="AA17" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="AB17" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="AC17" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="AD17" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="AE17" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="AF17" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="AG17" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="18" spans="1:35" ht="24" customHeight="1">
-      <c r="A18" s="9" t="s">
+      <c r="B18" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="AA18" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="AB18" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="AC18" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="AD18" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="AE18" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="AF18" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="AG18" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" ht="24" customHeight="1">
+      <c r="B19" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="AA19" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="AB19" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="AC19" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="AD19" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="AE19" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="AF19" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="AG19" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" ht="24" customHeight="1">
+      <c r="A21" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B21" s="9" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="24" customHeight="1">
-      <c r="A19" s="14" t="s">
+    <row r="22" spans="1:35" ht="24" customHeight="1">
+      <c r="A22" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B22" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="24" customHeight="1">
-      <c r="B20" s="10" t="s">
+    <row r="23" spans="1:35" ht="24" customHeight="1">
+      <c r="B23" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="24" customHeight="1">
-      <c r="B21" s="11"/>
-      <c r="AA21" s="6" t="s">
+    <row r="24" spans="1:35" ht="24" customHeight="1">
+      <c r="B24" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="AB21" s="6" t="s">
+      <c r="AA24" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB24" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="AC21" s="6" t="s">
+      <c r="AC24" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="AD21" s="6" t="s">
+      <c r="AD24" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="AE21" s="6" t="s">
+      <c r="AE24" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="AF21" s="6" t="s">
+      <c r="AF24" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="AG21" s="6" t="s">
+      <c r="AG24" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="AH21" s="6" t="s">
+      <c r="AH24" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="AI21" s="6" t="s">
+      <c r="AI24" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="24" customHeight="1">
-      <c r="A23" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="24" spans="1:35" ht="24" customHeight="1">
-      <c r="A24" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>282</v>
-      </c>
-    </row>
     <row r="25" spans="1:35" ht="24" customHeight="1">
-      <c r="B25" s="11"/>
+      <c r="B25" s="11" t="s">
+        <v>272</v>
+      </c>
       <c r="AA25" s="6" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="AB25" s="6" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="AC25" s="6" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="AD25" s="6" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="AE25" s="6" t="s">
-        <v>287</v>
+        <v>275</v>
+      </c>
+      <c r="AF25" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG25" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH25" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="AI25" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" ht="24" customHeight="1">
+      <c r="B26" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="AA26" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB26" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC26" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="AD26" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="AE26" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="AF26" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG26" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH26" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="AI26" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:35" ht="24" customHeight="1">
-      <c r="A27" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>289</v>
+      <c r="B27" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="AA27" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB27" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC27" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="AD27" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="AE27" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="AF27" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG27" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH27" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="AI27" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:35" ht="24" customHeight="1">
-      <c r="A28" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>291</v>
+      <c r="B28" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="AA28" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB28" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC28" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="AD28" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="AE28" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="AF28" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG28" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH28" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="AI28" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:35" ht="24" customHeight="1">
-      <c r="B29" s="8" t="s">
-        <v>50</v>
+      <c r="B29" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA29" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB29" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC29" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="AD29" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="AE29" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="AF29" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG29" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH29" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="AI29" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:35" ht="24" customHeight="1">
-      <c r="B30" s="11"/>
+      <c r="B30" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="AA30" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB30" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC30" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="AD30" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="AE30" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="AF30" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG30" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH30" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="AI30" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="32" spans="1:35" ht="24" customHeight="1">
       <c r="A32" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" ht="24" customHeight="1">
+      <c r="A33" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" ht="24" customHeight="1">
+      <c r="B34" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="AA34" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="AB34" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="AC34" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="AD34" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="AE34" s="6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" ht="24" customHeight="1">
+      <c r="A36" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" ht="24" customHeight="1">
+      <c r="A37" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" ht="24" customHeight="1">
+      <c r="B38" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" ht="24" customHeight="1">
+      <c r="B39" s="11"/>
+    </row>
+    <row r="41" spans="1:31" ht="24" customHeight="1">
+      <c r="A41" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B41" s="9" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="24" customHeight="1">
-      <c r="A33" s="14" t="s">
+    <row r="42" spans="1:31" ht="24" customHeight="1">
+      <c r="A42" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B42" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C42" s="10" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="24" customHeight="1">
-      <c r="B34" s="8" t="s">
+    <row r="43" spans="1:31" ht="24" customHeight="1">
+      <c r="B43" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="24" customHeight="1">
-      <c r="B35" s="11"/>
-    </row>
-    <row r="37" spans="1:3" ht="24" customHeight="1">
-      <c r="A37" s="9" t="s">
+    <row r="44" spans="1:31" ht="24" customHeight="1">
+      <c r="B44" s="11"/>
+    </row>
+    <row r="46" spans="1:31" ht="24" customHeight="1">
+      <c r="A46" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B46" s="9" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="24" customHeight="1">
-      <c r="A38" s="14" t="s">
+    <row r="47" spans="1:31" ht="24" customHeight="1">
+      <c r="A47" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B47" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C47" s="10" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="24" customHeight="1">
-      <c r="B39" s="8" t="s">
+    <row r="48" spans="1:31" ht="24" customHeight="1">
+      <c r="B48" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="24" customHeight="1">
-      <c r="B40" s="11"/>
-    </row>
-    <row r="42" spans="1:3" ht="24" customHeight="1">
-      <c r="A42" s="9" t="s">
+    <row r="49" spans="1:3" ht="24" customHeight="1">
+      <c r="B49" s="11" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="24" customHeight="1">
+      <c r="A51" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B51" s="9" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="24" customHeight="1">
-      <c r="A43" s="14" t="s">
+    <row r="52" spans="1:3" ht="24" customHeight="1">
+      <c r="A52" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B52" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C52" s="10" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="24" customHeight="1">
-      <c r="B44" s="8" t="s">
+    <row r="53" spans="1:3" ht="24" customHeight="1">
+      <c r="B53" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="24" customHeight="1">
-      <c r="B45" s="11"/>
-    </row>
-    <row r="47" spans="1:3" ht="24" customHeight="1">
-      <c r="A47" s="9" t="s">
+    <row r="54" spans="1:3" ht="24" customHeight="1">
+      <c r="B54" s="11"/>
+    </row>
+    <row r="56" spans="1:3" ht="24" customHeight="1">
+      <c r="A56" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B56" s="9" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="24" customHeight="1">
-      <c r="A48" s="14" t="s">
+    <row r="57" spans="1:3" ht="24" customHeight="1">
+      <c r="A57" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B57" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C57" s="10" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="24" customHeight="1">
-      <c r="B49" s="11"/>
+    <row r="58" spans="1:3" ht="24" customHeight="1">
+      <c r="B58" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="15"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:B19" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>AA16:AG16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
-      <formula1>AA21:AI21</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:B30" xr:uid="{00000000-0002-0000-0500-000001000000}">
+      <formula1>AA24:AI24</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
-      <formula1>AA25:AE25</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34" xr:uid="{00000000-0002-0000-0500-000002000000}">
+      <formula1>AA34:AE34</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3915,17 +4375,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -4099,22 +4559,25 @@
       <c r="B31" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="15"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -4192,7 +4655,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="24" customHeight="1">
+    <row r="17" spans="1:4" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
         <v>345</v>
       </c>
@@ -4200,7 +4663,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="24" customHeight="1">
+    <row r="18" spans="1:4" ht="24" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>347</v>
       </c>
@@ -4211,10 +4674,15 @@
         <v>349</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="24" customHeight="1">
-      <c r="B19" s="11"/>
-    </row>
-    <row r="21" spans="1:3" ht="24" customHeight="1">
+    <row r="19" spans="1:4" ht="24" customHeight="1">
+      <c r="B19" s="11">
+        <v>3.097</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="24" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>350</v>
       </c>
@@ -4222,7 +4690,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="24" customHeight="1">
+    <row r="22" spans="1:4" ht="24" customHeight="1">
       <c r="A22" s="14" t="s">
         <v>347</v>
       </c>
@@ -4233,10 +4701,10 @@
         <v>353</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="24" customHeight="1">
+    <row r="23" spans="1:4" ht="24" customHeight="1">
       <c r="B23" s="11"/>
     </row>
-    <row r="25" spans="1:3" ht="24" customHeight="1">
+    <row r="25" spans="1:4" ht="24" customHeight="1">
       <c r="A25" s="9" t="s">
         <v>354</v>
       </c>
@@ -4244,7 +4712,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="24" customHeight="1">
+    <row r="26" spans="1:4" ht="24" customHeight="1">
       <c r="A26" s="14" t="s">
         <v>347</v>
       </c>
@@ -4255,10 +4723,15 @@
         <v>357</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="24" customHeight="1">
-      <c r="B27" s="11"/>
-    </row>
-    <row r="30" spans="1:3" ht="24" customHeight="1">
+    <row r="27" spans="1:4" ht="24" customHeight="1">
+      <c r="B27" s="11">
+        <v>0.13469999999999999</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="24" customHeight="1">
       <c r="A30" s="12" t="s">
         <v>358</v>
       </c>
@@ -4266,7 +4739,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="24" customHeight="1">
+    <row r="31" spans="1:4" ht="24" customHeight="1">
       <c r="B31" s="13"/>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
@@ -4289,7 +4762,9 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
-      <c r="B35" s="11"/>
+      <c r="B35" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
       <c r="A37" s="9" t="s">
@@ -4311,7 +4786,9 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
-      <c r="B39" s="11"/>
+      <c r="B39" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1">
       <c r="A41" s="9" t="s">
@@ -4333,7 +4810,9 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
-      <c r="B43" s="11"/>
+      <c r="B43" s="11" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="46" spans="1:3" ht="24" customHeight="1">
       <c r="A46" s="12" t="s">
@@ -4368,7 +4847,9 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="24" customHeight="1">
-      <c r="B51" s="11"/>
+      <c r="B51" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:3" ht="24" customHeight="1">
       <c r="A53" s="9" t="s">
@@ -4390,7 +4871,9 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="24" customHeight="1">
-      <c r="B55" s="11"/>
+      <c r="B55" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:3" ht="24" customHeight="1">
       <c r="A57" s="9" t="s">
@@ -4412,7 +4895,9 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="24" customHeight="1">
-      <c r="B59" s="11"/>
+      <c r="B59" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="1:3" ht="24" customHeight="1">
       <c r="A62" s="12" t="s">
@@ -4452,7 +4937,9 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="178" customHeight="1">
-      <c r="B68" s="11"/>
+      <c r="B68" s="11" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="70" spans="1:3" ht="24" customHeight="1">
       <c r="A70" s="9" t="s">
@@ -4474,7 +4961,9 @@
       </c>
     </row>
     <row r="72" spans="1:3" ht="24" customHeight="1">
-      <c r="B72" s="11"/>
+      <c r="B72" s="11">
+        <v>15</v>
+      </c>
     </row>
     <row r="74" spans="1:3" ht="24" customHeight="1">
       <c r="A74" s="9" t="s">
@@ -4496,7 +4985,9 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="24" customHeight="1">
-      <c r="B76" s="11"/>
+      <c r="B76" s="11">
+        <v>14</v>
+      </c>
     </row>
     <row r="79" spans="1:3" ht="24" customHeight="1">
       <c r="A79" s="12" t="s">
@@ -4511,7 +5002,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="24" customHeight="1">
+    <row r="82" spans="1:4" ht="24" customHeight="1">
       <c r="A82" s="9" t="s">
         <v>404</v>
       </c>
@@ -4519,7 +5010,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="24" customHeight="1">
+    <row r="83" spans="1:4" ht="24" customHeight="1">
       <c r="A83" s="14" t="s">
         <v>43</v>
       </c>
@@ -4530,15 +5021,17 @@
         <v>406</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="24" customHeight="1">
+    <row r="84" spans="1:4" ht="24" customHeight="1">
       <c r="B84" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="178" customHeight="1">
-      <c r="B85" s="11"/>
-    </row>
-    <row r="87" spans="1:3" ht="24" customHeight="1">
+    <row r="85" spans="1:4" ht="178" customHeight="1">
+      <c r="B85" s="15" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="24" customHeight="1">
       <c r="A87" s="9" t="s">
         <v>407</v>
       </c>
@@ -4546,7 +5039,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="24" customHeight="1">
+    <row r="88" spans="1:4" ht="24" customHeight="1">
       <c r="A88" s="14" t="s">
         <v>83</v>
       </c>
@@ -4557,10 +5050,12 @@
         <v>410</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="24" customHeight="1">
-      <c r="B89" s="11"/>
-    </row>
-    <row r="91" spans="1:3" ht="24" customHeight="1">
+    <row r="89" spans="1:4" ht="24" customHeight="1">
+      <c r="B89" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="24" customHeight="1">
       <c r="A91" s="9" t="s">
         <v>411</v>
       </c>
@@ -4568,7 +5063,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="24" customHeight="1">
+    <row r="92" spans="1:4" ht="24" customHeight="1">
       <c r="A92" s="14" t="s">
         <v>78</v>
       </c>
@@ -4579,10 +5074,15 @@
         <v>414</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="24" customHeight="1">
-      <c r="B93" s="11"/>
-    </row>
-    <row r="95" spans="1:3" ht="24" customHeight="1">
+    <row r="93" spans="1:4" ht="24" customHeight="1">
+      <c r="B93" s="11">
+        <v>1</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="24" customHeight="1">
       <c r="A95" s="9" t="s">
         <v>415</v>
       </c>
@@ -4590,7 +5090,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="24" customHeight="1">
+    <row r="96" spans="1:4" ht="24" customHeight="1">
       <c r="A96" s="14" t="s">
         <v>83</v>
       </c>
@@ -4602,7 +5102,9 @@
       </c>
     </row>
     <row r="97" spans="1:3" ht="24" customHeight="1">
-      <c r="B97" s="11"/>
+      <c r="B97" s="11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="99" spans="1:3" ht="24" customHeight="1">
       <c r="A99" s="9" t="s">
@@ -4624,7 +5126,9 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="24" customHeight="1">
-      <c r="B101" s="11"/>
+      <c r="B101" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="103" spans="1:3" ht="24" customHeight="1">
       <c r="A103" s="9" t="s">
@@ -4646,56 +5150,21 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1">
-      <c r="B105" s="11"/>
+      <c r="B105" s="11">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="15">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
+  <phoneticPr fontId="15"/>
+  <dataValidations count="3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19 B27 B23" xr:uid="{00000000-0002-0000-0700-000000000000}">
+      <formula1>-1000000</formula1>
+      <formula2>1000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35 B101 B97 B89 B59 B55 B51 B39" xr:uid="{00000000-0002-0000-0700-000003000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B76">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B93">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B97">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B101">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B105">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72 B105 B93 B76" xr:uid="{00000000-0002-0000-0700-000008000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -4704,17 +5173,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:AN55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="24" customHeight="1">
@@ -4750,7 +5219,9 @@
       </c>
     </row>
     <row r="6" spans="1:39" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="8" spans="1:39" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -4777,7 +5248,9 @@
       </c>
     </row>
     <row r="11" spans="1:39" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="13" spans="1:39" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
@@ -4804,7 +5277,9 @@
       </c>
     </row>
     <row r="16" spans="1:39" ht="24" customHeight="1">
-      <c r="B16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>437</v>
+      </c>
       <c r="AA16" s="6" t="s">
         <v>437</v>
       </c>
@@ -4845,235 +5320,951 @@
         <v>449</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="24" customHeight="1">
-      <c r="A18" s="9" t="s">
+    <row r="17" spans="1:39" ht="24" customHeight="1">
+      <c r="B17" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="AA17" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="AB17" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="AC17" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="AD17" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="AE17" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="AF17" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="AG17" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="AH17" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AI17" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AJ17" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AK17" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AL17" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AM17" s="6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" ht="24" customHeight="1">
+      <c r="B18" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="AA18" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="AB18" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="AC18" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="AD18" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="AE18" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="AF18" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="AG18" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="AH18" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AI18" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AJ18" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AK18" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AL18" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AM18" s="6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" ht="24" customHeight="1">
+      <c r="B19" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="AA19" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="AB19" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="AC19" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="AD19" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="AE19" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="AF19" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="AG19" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="AH19" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AI19" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AJ19" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AK19" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AL19" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AM19" s="6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" ht="24" customHeight="1">
+      <c r="B20" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="AA20" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="AB20" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="AC20" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="AD20" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="AE20" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="AF20" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="AG20" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="AH20" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AI20" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AJ20" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AK20" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AL20" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AM20" s="6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" ht="24" customHeight="1">
+      <c r="B21" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="AA21" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="AB21" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="AC21" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="AE21" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="AF21" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="AG21" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="AH21" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AI21" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AJ21" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AK21" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AL21" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AM21" s="6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" ht="24" customHeight="1">
+      <c r="B22" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="AA22" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="AB22" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="AC22" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="AD22" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="AE22" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="AF22" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="AG22" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="AH22" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AI22" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AJ22" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AK22" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AL22" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AM22" s="6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" ht="24" customHeight="1">
+      <c r="B23" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="AA23" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="AB23" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="AC23" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="AD23" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="AE23" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="AF23" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="AG23" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="AH23" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AI23" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="AJ23" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="AK23" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="AL23" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AM23" s="6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" ht="24" customHeight="1">
+      <c r="A25" s="9" t="s">
         <v>450</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B25" s="9" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="24" customHeight="1">
-      <c r="A19" s="14" t="s">
+    <row r="26" spans="1:39" ht="24" customHeight="1">
+      <c r="A26" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B26" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C26" s="10" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="24" customHeight="1">
-      <c r="B20" s="10" t="s">
+    <row r="27" spans="1:39" ht="24" customHeight="1">
+      <c r="B27" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="24" customHeight="1">
-      <c r="B21" s="11"/>
-      <c r="AA21" s="6" t="s">
+    <row r="28" spans="1:39" ht="24" customHeight="1">
+      <c r="B28" s="11" t="s">
         <v>454</v>
       </c>
-      <c r="AB21" s="6" t="s">
+      <c r="AA28" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AB28" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="AC21" s="6" t="s">
+      <c r="AC28" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="AD21" s="6" t="s">
+      <c r="AD28" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="AE21" s="6" t="s">
+      <c r="AE28" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="AF21" s="6" t="s">
+      <c r="AF28" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="AG21" s="6" t="s">
+      <c r="AG28" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="AH21" s="6" t="s">
+      <c r="AH28" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="24" customHeight="1">
-      <c r="A23" s="9" t="s">
+    <row r="29" spans="1:39" ht="24" customHeight="1">
+      <c r="B29" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="AA29" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AB29" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AC29" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD29" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="AE29" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="AF29" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="AG29" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="AH29" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" ht="24" customHeight="1">
+      <c r="B30" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="AA30" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AB30" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AC30" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD30" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="AE30" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="AF30" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="AG30" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="AH30" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" ht="24" customHeight="1">
+      <c r="B31" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="AA31" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AB31" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AC31" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD31" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="AE31" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="AF31" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="AG31" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="AH31" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" ht="24" customHeight="1">
+      <c r="B32" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="AA32" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AB32" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AC32" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD32" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="AE32" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="AF32" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="AG32" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="AH32" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:35" ht="24" customHeight="1">
+      <c r="B33" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="AA33" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="AB33" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="AC33" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AD33" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="AE33" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="AF33" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="AG33" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="AH33" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:35" ht="24" customHeight="1">
+      <c r="A35" s="9" t="s">
         <v>460</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B35" s="9" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="24" customHeight="1">
-      <c r="A24" s="14" t="s">
+    <row r="36" spans="1:35" ht="24" customHeight="1">
+      <c r="A36" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B36" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C36" s="10" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="24" customHeight="1">
-      <c r="B25" s="10" t="s">
+    <row r="37" spans="1:35" ht="24" customHeight="1">
+      <c r="B37" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:35" ht="24" customHeight="1">
-      <c r="B26" s="11"/>
-      <c r="AA26" s="6" t="s">
+    <row r="38" spans="1:35" ht="24" customHeight="1">
+      <c r="B38" s="11" t="s">
         <v>464</v>
       </c>
-      <c r="AB26" s="6" t="s">
+      <c r="AA38" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="AB38" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="AC26" s="6" t="s">
+      <c r="AC38" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="AD26" s="6" t="s">
+      <c r="AD38" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="AE26" s="6" t="s">
+      <c r="AE38" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="AF26" s="6" t="s">
+      <c r="AF38" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="AG26" s="6" t="s">
+      <c r="AG38" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="AH26" s="6" t="s">
+      <c r="AH38" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="AI26" s="6" t="s">
+      <c r="AI38" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:35" ht="24" customHeight="1">
-      <c r="A28" s="9" t="s">
+    <row r="39" spans="1:35" ht="24" customHeight="1">
+      <c r="B39" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="AA39" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="AB39" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="AC39" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="AD39" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="AE39" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="AF39" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="AG39" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="AH39" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AI39" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" ht="24" customHeight="1">
+      <c r="B40" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="AA40" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="AB40" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="AC40" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="AD40" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="AE40" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="AF40" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="AG40" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="AH40" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AI40" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35" ht="24" customHeight="1">
+      <c r="B41" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="AA41" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="AB41" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="AC41" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="AD41" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="AE41" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="AF41" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="AG41" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="AH41" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AI41" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35" ht="24" customHeight="1">
+      <c r="A43" s="9" t="s">
         <v>472</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B43" s="9" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="24" customHeight="1">
-      <c r="A29" s="14" t="s">
+    <row r="44" spans="1:35" ht="24" customHeight="1">
+      <c r="A44" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B44" s="10" t="s">
         <v>474</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C44" s="10" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="30" spans="1:35" ht="24" customHeight="1">
-      <c r="B30" s="10" t="s">
+    <row r="45" spans="1:35" ht="24" customHeight="1">
+      <c r="B45" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:35" ht="24" customHeight="1">
-      <c r="B31" s="11"/>
-      <c r="AA31" s="6" t="s">
+    <row r="46" spans="1:35" ht="24" customHeight="1">
+      <c r="B46" s="11" t="s">
         <v>476</v>
       </c>
-      <c r="AB31" s="6" t="s">
+      <c r="AA46" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AB46" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="AC31" s="6" t="s">
+      <c r="AC46" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="AD31" s="6" t="s">
+      <c r="AD46" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:40" ht="24" customHeight="1">
-      <c r="A33" s="9" t="s">
+    <row r="47" spans="1:35" ht="24" customHeight="1">
+      <c r="B47" s="11" t="s">
+        <v>478</v>
+      </c>
+      <c r="AA47" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AB47" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AC47" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD47" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:40" ht="24" customHeight="1">
+      <c r="A49" s="9" t="s">
         <v>479</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B49" s="9" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="34" spans="1:40" ht="24" customHeight="1">
-      <c r="A34" s="14" t="s">
+    <row r="50" spans="1:40" ht="24" customHeight="1">
+      <c r="A50" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B50" s="10" t="s">
         <v>481</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C50" s="10" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="35" spans="1:40" ht="24" customHeight="1">
-      <c r="B35" s="10" t="s">
+    <row r="51" spans="1:40" ht="24" customHeight="1">
+      <c r="B51" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:40" ht="24" customHeight="1">
-      <c r="B36" s="11"/>
-      <c r="AA36" s="6" t="s">
+    <row r="52" spans="1:40" ht="24" customHeight="1">
+      <c r="B52" s="11" t="s">
         <v>483</v>
       </c>
-      <c r="AB36" s="6" t="s">
+      <c r="AA52" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="AB52" s="6" t="s">
         <v>484</v>
       </c>
-      <c r="AC36" s="6" t="s">
+      <c r="AC52" s="6" t="s">
         <v>485</v>
       </c>
-      <c r="AD36" s="6" t="s">
+      <c r="AD52" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="AE36" s="6" t="s">
+      <c r="AE52" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="AF36" s="6" t="s">
+      <c r="AF52" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="AG36" s="6" t="s">
+      <c r="AG52" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="AH36" s="6" t="s">
+      <c r="AH52" s="6" t="s">
         <v>489</v>
       </c>
-      <c r="AI36" s="6" t="s">
+      <c r="AI52" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="AJ36" s="6" t="s">
+      <c r="AJ52" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="AK36" s="6" t="s">
+      <c r="AK52" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="AL36" s="6" t="s">
+      <c r="AL52" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="AM36" s="6" t="s">
+      <c r="AM52" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="AN36" s="6" t="s">
+      <c r="AN52" s="6" t="s">
         <v>65</v>
       </c>
     </row>
+    <row r="53" spans="1:40" ht="24" customHeight="1">
+      <c r="B53" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="AA53" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="AB53" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="AC53" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="AD53" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="AE53" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="AF53" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="AG53" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="AH53" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="AI53" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="AJ53" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="AK53" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="AL53" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="AM53" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="AN53" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:40" ht="24" customHeight="1">
+      <c r="B54" s="11" t="s">
+        <v>489</v>
+      </c>
+      <c r="AA54" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="AB54" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="AC54" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="AD54" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="AE54" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="AF54" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="AG54" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="AH54" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="AI54" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="AJ54" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="AK54" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="AL54" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="AM54" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="AN54" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:40" ht="24" customHeight="1">
+      <c r="B55" s="11" t="s">
+        <v>490</v>
+      </c>
+      <c r="AA55" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="AB55" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="AC55" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="AD55" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="AE55" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="AF55" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="AG55" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="AH55" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="AI55" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="AJ55" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="AK55" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="AL55" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="AM55" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="AN55" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="15"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:B23" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>AA16:AM16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
-      <formula1>AA21:AH21</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28:B33" xr:uid="{00000000-0002-0000-0800-000001000000}">
+      <formula1>AA28:AH28</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26">
-      <formula1>AA26:AI26</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38:B41" xr:uid="{00000000-0002-0000-0800-000002000000}">
+      <formula1>AA38:AI38</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31">
-      <formula1>AA31:AD31</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B46:B47" xr:uid="{00000000-0002-0000-0800-000003000000}">
+      <formula1>AA46:AD46</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36">
-      <formula1>AA36:AN36</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B52:B55" xr:uid="{00000000-0002-0000-0800-000004000000}">
+      <formula1>AA52:AN52</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>